<commit_message>
fix tix + loc
</commit_message>
<xml_diff>
--- a/sample_location.xlsx
+++ b/sample_location.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>locid</t>
   </si>
@@ -36,19 +36,31 @@
     <t>postal</t>
   </si>
   <si>
-    <t>area</t>
-  </si>
-  <si>
     <t>lat</t>
   </si>
   <si>
     <t>lng</t>
   </si>
   <si>
-    <t>location 1</t>
-  </si>
-  <si>
     <t>custom street 1st</t>
+  </si>
+  <si>
+    <t>lnk</t>
+  </si>
+  <si>
+    <t>Astinet</t>
+  </si>
+  <si>
+    <t>bw</t>
+  </si>
+  <si>
+    <t>2 MB</t>
+  </si>
+  <si>
+    <t>LOC123</t>
+  </si>
+  <si>
+    <t>location 123</t>
   </si>
 </sst>
 </file>
@@ -387,15 +399,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C2"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -421,18 +437,27 @@
         <v>7</v>
       </c>
       <c r="I1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1234</v>
-      </c>
-      <c r="B2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="I2" t="s">
         <v>10</v>
+      </c>
+      <c r="J2" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>